<commit_message>
default values for options
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\Comsc-131\Comsc-131-Project-Team-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C54B3A8-FDF3-438C-91CB-214248516C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C460B67-1533-40B2-8CB5-4B3C0FB2254C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1057,8 +1057,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:Q11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8:W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1419,13 +1419,13 @@
         <v>4</v>
       </c>
       <c r="E7" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F7" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="42" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated finished gantt, update page, final commit
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Documents\Comsc-131\Comsc-131-Project-Team-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C460B67-1533-40B2-8CB5-4B3C0FB2254C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19549C93-F41C-4064-B62D-0B274D591312}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Project Planner</t>
   </si>
@@ -156,60 +156,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Feature 09</t>
-  </si>
-  <si>
-    <t>Feature 10</t>
-  </si>
-  <si>
-    <t>Feature 11</t>
-  </si>
-  <si>
-    <t>Feature 12</t>
-  </si>
-  <si>
-    <t>Feature 13</t>
-  </si>
-  <si>
-    <t>Feature 14</t>
-  </si>
-  <si>
-    <t>Feature 15</t>
-  </si>
-  <si>
-    <t>Feature 16</t>
-  </si>
-  <si>
-    <t>Feature 17</t>
-  </si>
-  <si>
-    <t>Feature 18</t>
-  </si>
-  <si>
-    <t>Feature 19</t>
-  </si>
-  <si>
-    <t>Feature 20</t>
-  </si>
-  <si>
-    <t>Feature 21</t>
-  </si>
-  <si>
-    <t>Feature 22</t>
-  </si>
-  <si>
-    <t>Feature 23</t>
-  </si>
-  <si>
-    <t>Feature 24</t>
-  </si>
-  <si>
-    <t>Feature 25</t>
-  </si>
-  <si>
-    <t>Feature 26</t>
-  </si>
-  <si>
     <t>Login/logout</t>
   </si>
   <si>
@@ -232,6 +178,21 @@
   </si>
   <si>
     <t>Account public/private setting on an options menu webpage</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>class faq</t>
+  </si>
+  <si>
+    <t>share notes (markdown)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pomodoro timer</t>
+  </si>
+  <si>
+    <t>classroom invite link</t>
   </si>
 </sst>
 </file>
@@ -274,17 +235,20 @@
       <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="7"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1058,7 +1022,7 @@
   <dimension ref="B1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8:W9"/>
+      <selection activeCell="AR11" sqref="AR11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1334,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1382,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
@@ -1390,7 +1354,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1402,7 +1366,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G6" s="8">
         <v>1</v>
@@ -1410,7 +1374,7 @@
     </row>
     <row r="7" spans="2:67" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -1430,7 +1394,7 @@
     </row>
     <row r="8" spans="2:67" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C8" s="7">
         <v>11</v>
@@ -1439,18 +1403,18 @@
         <v>6</v>
       </c>
       <c r="E8" s="7">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F8" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7">
         <v>11</v>
@@ -1459,18 +1423,18 @@
         <v>6</v>
       </c>
       <c r="E9" s="7">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F9" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7">
         <v>6</v>
@@ -1479,38 +1443,38 @@
         <v>6</v>
       </c>
       <c r="E10" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F10" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:67" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C11" s="7">
         <v>6</v>
       </c>
       <c r="D11" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E11" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F11" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G11" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C12" s="7">
         <v>11</v>
@@ -1519,50 +1483,50 @@
         <v>6</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F12" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D13" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E13" s="7">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F13" s="7">
         <v>6</v>
       </c>
       <c r="G13" s="8">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C14" s="7">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D14" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" s="7">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F14" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14" s="8">
         <v>1</v>
@@ -1570,323 +1534,167 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="9">
         <v>17</v>
       </c>
-      <c r="C15" s="9">
-        <v>6</v>
-      </c>
       <c r="D15" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E15" s="7">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F15" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" s="8">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C16" s="7">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D16" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="7">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F16" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G16" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C17" s="7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D17" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E17" s="7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F17" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G17" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="7">
-        <v>9</v>
-      </c>
-      <c r="D18" s="7">
-        <v>3</v>
-      </c>
-      <c r="E18" s="7">
-        <v>9</v>
-      </c>
-      <c r="F18" s="7">
-        <v>1</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0</v>
-      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="7">
-        <v>9</v>
-      </c>
-      <c r="D19" s="7">
-        <v>4</v>
-      </c>
-      <c r="E19" s="7">
-        <v>8</v>
-      </c>
-      <c r="F19" s="7">
-        <v>5</v>
-      </c>
-      <c r="G19" s="8">
-        <v>0.01</v>
-      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="7">
-        <v>10</v>
-      </c>
-      <c r="D20" s="7">
-        <v>5</v>
-      </c>
-      <c r="E20" s="7">
-        <v>10</v>
-      </c>
-      <c r="F20" s="7">
-        <v>3</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0.8</v>
-      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="7">
-        <v>11</v>
-      </c>
-      <c r="D21" s="7">
-        <v>2</v>
-      </c>
-      <c r="E21" s="7">
-        <v>11</v>
-      </c>
-      <c r="F21" s="7">
-        <v>5</v>
-      </c>
-      <c r="G21" s="8">
-        <v>0</v>
-      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="7">
-        <v>12</v>
-      </c>
-      <c r="D22" s="7">
-        <v>6</v>
-      </c>
-      <c r="E22" s="7">
-        <v>12</v>
-      </c>
-      <c r="F22" s="7">
-        <v>7</v>
-      </c>
-      <c r="G22" s="8">
-        <v>0</v>
-      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="7">
-        <v>12</v>
-      </c>
-      <c r="D23" s="7">
-        <v>1</v>
-      </c>
-      <c r="E23" s="7">
-        <v>12</v>
-      </c>
-      <c r="F23" s="7">
-        <v>5</v>
-      </c>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="7">
-        <v>14</v>
-      </c>
-      <c r="D24" s="7">
-        <v>5</v>
-      </c>
-      <c r="E24" s="7">
-        <v>14</v>
-      </c>
-      <c r="F24" s="7">
-        <v>6</v>
-      </c>
-      <c r="G24" s="8">
-        <v>0</v>
-      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="7">
-        <v>14</v>
-      </c>
-      <c r="D25" s="7">
-        <v>8</v>
-      </c>
-      <c r="E25" s="7">
-        <v>14</v>
-      </c>
-      <c r="F25" s="7">
-        <v>2</v>
-      </c>
-      <c r="G25" s="8">
-        <v>0.44</v>
-      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="7">
-        <v>14</v>
-      </c>
-      <c r="D26" s="7">
-        <v>7</v>
-      </c>
-      <c r="E26" s="7">
-        <v>14</v>
-      </c>
-      <c r="F26" s="7">
-        <v>3</v>
-      </c>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="7">
-        <v>15</v>
-      </c>
-      <c r="D27" s="7">
-        <v>4</v>
-      </c>
-      <c r="E27" s="7">
-        <v>15</v>
-      </c>
-      <c r="F27" s="7">
-        <v>8</v>
-      </c>
-      <c r="G27" s="8">
-        <v>0.12</v>
-      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="7">
-        <v>15</v>
-      </c>
-      <c r="D28" s="7">
-        <v>5</v>
-      </c>
-      <c r="E28" s="7">
-        <v>15</v>
-      </c>
-      <c r="F28" s="7">
-        <v>3</v>
-      </c>
-      <c r="G28" s="8">
-        <v>0.05</v>
-      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="7">
-        <v>15</v>
-      </c>
-      <c r="D29" s="7">
-        <v>8</v>
-      </c>
-      <c r="E29" s="7">
-        <v>15</v>
-      </c>
-      <c r="F29" s="7">
-        <v>5</v>
-      </c>
-      <c r="G29" s="8">
-        <v>0</v>
-      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="7">
-        <v>16</v>
-      </c>
-      <c r="D30" s="7">
-        <v>28</v>
-      </c>
-      <c r="E30" s="7">
-        <v>16</v>
-      </c>
-      <c r="F30" s="7">
-        <v>30</v>
-      </c>
-      <c r="G30" s="8">
-        <v>0.5</v>
-      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>